<commit_message>
Update foreign key position
</commit_message>
<xml_diff>
--- a/test/xls/ConstStatic.xlsx
+++ b/test/xls/ConstStatic.xlsx
@@ -1,94 +1,172 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28695" windowHeight="12630"/>
   </bookViews>
   <sheets>
     <sheet name="ConstStatic" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
+  <si>
+    <t>ClassName</t>
+  </si>
+  <si>
+    <t>ConstStatic</t>
+  </si>
+  <si>
+    <t>ClassDescription</t>
+  </si>
+  <si>
+    <t>常量静态表</t>
+  </si>
+  <si>
+    <t>ClassGroup</t>
+  </si>
+  <si>
+    <t>InitializeStatic</t>
+  </si>
+  <si>
+    <t>FieldName</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>CatTriggerTime</t>
+  </si>
+  <si>
+    <t>MaxRestoreCardNum</t>
+  </si>
+  <si>
+    <t>FieldDescription</t>
+  </si>
+  <si>
+    <t>猫获取经验触发时间间隔(小时)</t>
+  </si>
+  <si>
+    <t>最多收集卡片数量</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>Uniqueness</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
   <si>
     <t>Client</t>
   </si>
   <si>
-    <t>Server</t>
-  </si>
-  <si>
-    <t>Required</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Uniqueness</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>FieldDescription</t>
-  </si>
-  <si>
-    <t>FieldName</t>
-  </si>
-  <si>
-    <t>InitializeStatic</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ClassGroup</t>
-  </si>
-  <si>
-    <t>常量静态表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ClassDescription</t>
-  </si>
-  <si>
-    <t>ConstStatic</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ClassName</t>
-  </si>
-  <si>
-    <t>CatTriggerTime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>猫获取经验触发时间间隔(小时)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MaxRestoreCardNum</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最多收集卡片数量</t>
+    <t>BgSoundName_ARRoom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BgSoundName_3DRoom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BgSoundName_FittingRoom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ar房间背景音乐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3D房间背景音乐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>试衣间背景音乐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>audio_bg_arroom</t>
+  </si>
+  <si>
+    <t>audio_bg_3droom</t>
+  </si>
+  <si>
+    <t>audio_bg_fittingroom</t>
+  </si>
+  <si>
+    <t>audio_common_getcard</t>
+  </si>
+  <si>
+    <t>audio_common_click</t>
+  </si>
+  <si>
+    <t>audio_common_getscard</t>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ommonSound_GetCoin</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CommonSound_GetCard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CommonSound_GetSunperCard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CommonSound_OpenView</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得金币音效</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得卡片音效</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>打开界面音效</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得超级卡片音效</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -96,16 +174,24 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -132,11 +218,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -146,9 +233,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -407,140 +491,269 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="10" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
+      <pane xSplit="2" ySplit="10" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="15.125" customWidth="1"/>
     <col min="3" max="3" width="26.625" customWidth="1"/>
+    <col min="4" max="4" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" t="b">
-        <v>1</v>
-      </c>
-      <c r="C8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" t="b">
-        <v>1</v>
-      </c>
-      <c r="C9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
       <c r="B10" t="b">
         <v>1</v>
       </c>
@@ -550,8 +763,29 @@
       <c r="D10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>1</v>
       </c>
@@ -561,10 +795,31 @@
       <c r="D11">
         <v>60</v>
       </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>